<commit_message>
create DummyClient, PacketMaker bug fix
</commit_message>
<xml_diff>
--- a/PacketRule.xlsx
+++ b/PacketRule.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4561EDF9-DEEB-4B33-A021-A98E28EF220C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F448EB5B-D2FA-473C-82C6-2F4B2198168D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11355" yWindow="1935" windowWidth="17445" windowHeight="11445" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11355" yWindow="1935" windowWidth="17445" windowHeight="11445" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PacketData" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="PacketFactory" sheetId="4" r:id="rId4"/>
     <sheet name="ClientPacketClass" sheetId="5" r:id="rId5"/>
     <sheet name="ClientPacketHeader" sheetId="6" r:id="rId6"/>
-    <sheet name="ClilentPacketFactory" sheetId="7" r:id="rId7"/>
+    <sheet name="ClientPacketFactory" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -711,7 +711,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -899,7 +899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC879773-F0B2-4EBA-8D80-2502C10F0DF0}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1229,7 +1229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA9B25F-1C6C-46DC-99A8-259167291EEC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>